<commit_message>
Finally the DB is FULL :'D
</commit_message>
<xml_diff>
--- a/Information/LISTA DISTINCIONES RFC 2018.xlsx
+++ b/Information/LISTA DISTINCIONES RFC 2018.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\OrganizeAnEvent\Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41790690-67C0-4201-9C85-CF9074E514A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21285" windowHeight="12255"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21285" windowHeight="12255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LISTADO COMPLETO" sheetId="5" r:id="rId1"/>
@@ -3682,7 +3683,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4309,7 +4310,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 101" descr="LIC"/>
+        <xdr:cNvPr id="2" name="Imagen 101" descr="LIC">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -4364,7 +4371,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 162" descr="ING"/>
+        <xdr:cNvPr id="3" name="Imagen 162" descr="ING">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -4419,7 +4432,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CuadroTexto 3"/>
+        <xdr:cNvPr id="4" name="CuadroTexto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4571,7 +4590,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CuadroTexto 4"/>
+        <xdr:cNvPr id="5" name="CuadroTexto 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4714,7 +4739,7 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-MX" sz="1300" b="0" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+            <a:rPr lang="es-MX" sz="1300" b="0" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -4836,7 +4861,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CuadroTexto 5"/>
+        <xdr:cNvPr id="6" name="CuadroTexto 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4918,7 +4949,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CuadroTexto 6"/>
+        <xdr:cNvPr id="7" name="CuadroTexto 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5103,7 +5140,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="CuadroTexto 7"/>
+        <xdr:cNvPr id="8" name="CuadroTexto 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5291,7 +5334,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CuadroTexto 8"/>
+        <xdr:cNvPr id="9" name="CuadroTexto 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5455,7 +5504,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="CuadroTexto 9"/>
+        <xdr:cNvPr id="10" name="CuadroTexto 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5580,7 +5635,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="CuadroTexto 10"/>
+        <xdr:cNvPr id="11" name="CuadroTexto 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5787,7 +5848,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="CuadroTexto 11"/>
+        <xdr:cNvPr id="12" name="CuadroTexto 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5981,7 +6048,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="CuadroTexto 12"/>
+        <xdr:cNvPr id="13" name="CuadroTexto 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -6356,11 +6429,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1238"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A833" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="F1238" sqref="F18:F1238"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A1188" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C1238" sqref="C1238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>

</xml_diff>